<commit_message>
Added resting heart rate
Added a resting heart rate generator, its related data and documentation.
</commit_message>
<xml_diff>
--- a/Background_Data/instruction_level.xlsx
+++ b/Background_Data/instruction_level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Git Repositories\UFTM-BioStat-DataBase\Background_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1D692A-61CD-4FB8-8F72-BEC7356C31DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6885F36D-A574-4BBB-8CDE-196F113C4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6C86C4E-3FA0-4625-B6AD-B93375B45EA5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E6C86C4E-3FA0-4625-B6AD-B93375B45EA5}"/>
   </bookViews>
   <sheets>
     <sheet name="14_sex" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="41">
   <si>
     <t>state</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>instruction_level_prova</t>
   </si>
 </sst>
 </file>
@@ -512,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{306051E5-22E0-4F72-AC7E-4871449C6497}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6186,8 +6189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219931F3-2827-43FD-A12F-C35DC7DF3704}">
   <dimension ref="A1:D190"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6197,7 +6200,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
         <v>38</v>

</xml_diff>